<commit_message>
added itterate function, changed getdatafromcell.
</commit_message>
<xml_diff>
--- a/Excel_read_serialnumber/Excel/WorkbookPy.xlsx
+++ b/Excel_read_serialnumber/Excel/WorkbookPy.xlsx
@@ -364,11 +364,6 @@
       <c r="A3" s="1" t="n">
         <v>60257</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>19011200020001</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">

</xml_diff>